<commit_message>
updated bcrbq, bgdpbes, bpmccs, crbq, dpbes, pmccs, raf
</commit_message>
<xml_diff>
--- a/InputData/elec/DPbES/Dispatch Priority by Elec Source.xlsx
+++ b/InputData/elec/DPbES/Dispatch Priority by Elec Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\DPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\elec\DPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C8F9E5-B6A6-4447-82DB-CD37DB5FC402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555FE573-E3F5-47B8-9548-34E99EBB0256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8070" yWindow="615" windowWidth="20025" windowHeight="16860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -198,7 +198,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -522,7 +521,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="1"/>
@@ -570,8 +569,8 @@
   </sheetPr>
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:AE14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,94 +1063,94 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update guaranteed dispatch and dpbes
</commit_message>
<xml_diff>
--- a/InputData/elec/DPbES/Dispatch Priority by Elec Source.xlsx
+++ b/InputData/elec/DPbES/Dispatch Priority by Elec Source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\elec\DPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555FE573-E3F5-47B8-9548-34E99EBB0256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EAF072-5AAA-465F-82E9-1432EBE70DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8070" yWindow="615" windowWidth="20025" windowHeight="16860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -570,7 +570,7 @@
   <dimension ref="A1:AI25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,94 +1633,94 @@
         <v>6</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adjust guaranteed dispatch priority
</commit_message>
<xml_diff>
--- a/InputData/elec/DPbES/Dispatch Priority by Elec Source.xlsx
+++ b/InputData/elec/DPbES/Dispatch Priority by Elec Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\DPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB717C7-2A8A-4BEC-A558-3F2E3A1EA905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819173F8-314B-44DF-BEC5-13FEFB698E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -569,8 +569,8 @@
   </sheetPr>
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:AE10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,94 +683,94 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
@@ -2298,94 +2298,94 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>